<commit_message>
New menu sections + nutrition labels
</commit_message>
<xml_diff>
--- a/files/menus/mtbenson_market/grabngo_mtbenson.xlsx
+++ b/files/menus/mtbenson_market/grabngo_mtbenson.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ollip\Documents\!!ProjectFiles\ezrab_feedbc\files\menus\mtbenson_market\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DEA5FA1-376B-41DD-A5F9-A8FB838D2CA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{A73B996D-920A-4A61-9AEB-EBF482D7368C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10785" yWindow="2265" windowWidth="24825" windowHeight="14220" xr2:uid="{F9466112-CF85-4C07-B090-DE232439FD19}"/>
+    <workbookView xWindow="15705" yWindow="3615" windowWidth="24345" windowHeight="16710" xr2:uid="{F9466112-CF85-4C07-B090-DE232439FD19}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="grabngo_mtbenson" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="30">
   <si>
     <t>Ingredients</t>
   </si>
@@ -53,62 +53,86 @@
     <t>nutritionLabel</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>waffles</t>
-  </si>
-  <si>
-    <t>Egg, Sausage</t>
-  </si>
-  <si>
-    <t>Potato</t>
-  </si>
-  <si>
-    <t>VGN, GF, DF</t>
-  </si>
-  <si>
-    <t>Turkey / Bacon / Cheddar Cheese / Lettuce / Tomato / Garlic Aioli</t>
-  </si>
-  <si>
-    <t>Turkey / Swiss Cheese / Roasted Onion / Tomato / Cucumber / Mixed Greens / Spicy Mayo</t>
-  </si>
-  <si>
-    <t>Falafel / Feta / Red Onion / Cucumber / Mixed Greens / Tomato / Tzatziki</t>
-  </si>
-  <si>
     <t>Allergens</t>
   </si>
   <si>
-    <t>Wheat, sulphites, egg.</t>
-  </si>
-  <si>
-    <t>No known priority allergens</t>
-  </si>
-  <si>
-    <t>GF</t>
-  </si>
-  <si>
-    <t>GF,VEG</t>
-  </si>
-  <si>
-    <t>Fruit Cup</t>
-  </si>
-  <si>
-    <t>Vegetable &amp; Dip</t>
-  </si>
-  <si>
     <t>Falafel &amp; Dip</t>
   </si>
   <si>
     <t>LeaveEmpty</t>
+  </si>
+  <si>
+    <t>Protein Pack</t>
+  </si>
+  <si>
+    <t>Vegetarian Protein Pack</t>
+  </si>
+  <si>
+    <t>Seasonal Cut Fruit</t>
+  </si>
+  <si>
+    <t>Chicken Gyoza</t>
+  </si>
+  <si>
+    <t>Shimp Gyoza</t>
+  </si>
+  <si>
+    <t>Packaged Curry Meal Small</t>
+  </si>
+  <si>
+    <t>Yogurt Parfait</t>
+  </si>
+  <si>
+    <t>Overnight Oats</t>
+  </si>
+  <si>
+    <t>Chia Pudding</t>
+  </si>
+  <si>
+    <t>Portioned Eggs (2)</t>
+  </si>
+  <si>
+    <t>Seasonal Fruit</t>
+  </si>
+  <si>
+    <t>Shrimp</t>
+  </si>
+  <si>
+    <t>Hard boiled eggs</t>
+  </si>
+  <si>
+    <t>needed</t>
+  </si>
+  <si>
+    <t>Salami / Cheddar Cheese / Dates / Melba Toast / Chocolate</t>
+  </si>
+  <si>
+    <t>Cucumber / Carrot / Tomato / Eggs / Cheddar Cheese / Nuts</t>
+  </si>
+  <si>
+    <t>Falafel / Cucumber / Tzatziki</t>
+  </si>
+  <si>
+    <t>Chicken / Vegetable</t>
+  </si>
+  <si>
+    <t>Basmati Rice / Butter Chicken sauce / Roasted Chicken</t>
+  </si>
+  <si>
+    <t>Yogurt / Granola / Seasonal Fruit</t>
+  </si>
+  <si>
+    <t>Milk / Oats / Chia Seed / Yogurt / Vanilla / Seasonal Fruit</t>
+  </si>
+  <si>
+    <t>Milk / Chia Seeds / Honey / Seasonal Fruit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,6 +142,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -143,10 +174,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -166,8 +219,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A32FF9D1-238C-44C9-AD02-5D859735230E}" name="Table3" displayName="Table3" ref="A1:G5" totalsRowShown="0">
-  <autoFilter ref="A1:G5" xr:uid="{A32FF9D1-238C-44C9-AD02-5D859735230E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A32FF9D1-238C-44C9-AD02-5D859735230E}" name="Table3" displayName="Table3" ref="A1:G23" totalsRowShown="0">
+  <autoFilter ref="A1:G23" xr:uid="{A32FF9D1-238C-44C9-AD02-5D859735230E}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{AA44CCDF-F9E2-4FB6-9AED-85FE3A3C6008}" name="ItemName"/>
     <tableColumn id="2" xr3:uid="{9D7FC130-DF66-4465-8F0B-6015043C6AA1}" name="Ingredients"/>
@@ -478,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2E4FEC9-4E15-443B-89A8-5C76E19963E8}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,7 +555,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -514,67 +567,227 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="B9" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="B11" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B12" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>6</v>
+      <c r="C12" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>